<commit_message>
earnings per share pivot table updates
</commit_message>
<xml_diff>
--- a/earnings_per_share_pivot_table.xlsx
+++ b/earnings_per_share_pivot_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1507" documentId="11_2869E2F47DC3CC36B52C4C8BBD6D1A1B7879E71B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D289DC92-2FD9-4A42-8A1C-E6C7667C572E}"/>
+  <xr:revisionPtr revIDLastSave="1360" documentId="11_2869E2F47DC3CC36B52C4CCA0D6C18477979E71B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{303021E6-5CCA-46DB-8B95-71DE07AB736E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1420,7 +1420,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1436,6 +1436,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA9D08E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3B7FCD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1467,13 +1473,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1874,7 +1881,7 @@
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>0</v>
       </c>
       <c r="G5" s="3">
@@ -1934,7 +1941,7 @@
       <c r="I8" s="3">
         <v>1.26</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1959,7 +1966,7 @@
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="4">
         <v>0</v>
       </c>
       <c r="G10" s="3">
@@ -2036,7 +2043,7 @@
       <c r="H14" s="3">
         <v>3.34</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2061,7 +2068,7 @@
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="4">
         <v>0</v>
       </c>
       <c r="G16" s="3">
@@ -2104,7 +2111,7 @@
       <c r="I18" s="3">
         <v>2.08</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2121,7 +2128,7 @@
       <c r="I19" s="3">
         <v>2.0699999999999998</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2197,7 +2204,7 @@
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="4">
         <v>0</v>
       </c>
       <c r="H24" s="3">
@@ -2206,7 +2213,7 @@
       <c r="I24" s="3">
         <v>1.6</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2223,7 +2230,7 @@
       <c r="I25" s="3">
         <v>0.68</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2291,7 +2298,7 @@
       <c r="I29" s="3">
         <v>9.15</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2342,7 +2349,7 @@
       <c r="I32" s="3">
         <v>1.28</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2359,7 +2366,7 @@
       <c r="I33" s="3">
         <v>3.93</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2427,7 +2434,7 @@
       <c r="I37" s="2">
         <v>-13.18</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2520,10 +2527,10 @@
       <c r="A43" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
+      <c r="I43" s="4">
+        <v>0</v>
+      </c>
+      <c r="J43" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2531,7 +2538,7 @@
       <c r="A44" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="4">
         <v>0</v>
       </c>
       <c r="G44" s="3">
@@ -2571,10 +2578,10 @@
       <c r="G46" s="3">
         <v>4.91</v>
       </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
+      <c r="H46" s="4">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2625,7 +2632,7 @@
       <c r="I49" s="3">
         <v>7.52</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2642,7 +2649,7 @@
       <c r="H50" s="3">
         <v>0.36</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2727,7 +2734,7 @@
       <c r="I55" s="3">
         <v>1.8</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2761,7 +2768,7 @@
       <c r="I57" s="2">
         <v>-4.49</v>
       </c>
-      <c r="J57">
+      <c r="J57" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2778,7 +2785,7 @@
       <c r="I58" s="3">
         <v>15.38</v>
       </c>
-      <c r="J58">
+      <c r="J58" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2863,7 +2870,7 @@
       <c r="I63" s="3">
         <v>2.72</v>
       </c>
-      <c r="J63">
+      <c r="J63" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2948,7 +2955,7 @@
       <c r="I68" s="3">
         <v>3.54</v>
       </c>
-      <c r="J68">
+      <c r="J68" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3016,7 +3023,7 @@
       <c r="I72" s="3">
         <v>2.2599999999999998</v>
       </c>
-      <c r="J72">
+      <c r="J72" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3033,7 +3040,7 @@
       <c r="I73" s="3">
         <v>2.02</v>
       </c>
-      <c r="J73">
+      <c r="J73" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3072,10 +3079,10 @@
       <c r="A76" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F76">
-        <v>0</v>
-      </c>
-      <c r="G76">
+      <c r="F76" s="4">
+        <v>0</v>
+      </c>
+      <c r="G76" s="4">
         <v>0</v>
       </c>
       <c r="H76" s="3">
@@ -3149,7 +3156,7 @@
       <c r="I80" s="2">
         <v>-2.4300000000000002</v>
       </c>
-      <c r="J80">
+      <c r="J80" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3234,7 +3241,7 @@
       <c r="I85" s="3">
         <v>2.93</v>
       </c>
-      <c r="J85">
+      <c r="J85" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3268,7 +3275,7 @@
       <c r="I87" s="3">
         <v>15.3</v>
       </c>
-      <c r="J87">
+      <c r="J87" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3285,7 +3292,7 @@
       <c r="I88" s="3">
         <v>7.86</v>
       </c>
-      <c r="J88">
+      <c r="J88" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3302,7 +3309,7 @@
       <c r="I89" s="3">
         <v>1.9</v>
       </c>
-      <c r="J89">
+      <c r="J89" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3401,7 +3408,7 @@
       <c r="H95" s="3">
         <v>5.61</v>
       </c>
-      <c r="I95">
+      <c r="I95" s="4">
         <v>0</v>
       </c>
       <c r="J95" s="3">
@@ -3429,16 +3436,16 @@
       <c r="A97" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B97">
-        <v>0</v>
-      </c>
-      <c r="C97">
-        <v>0</v>
-      </c>
-      <c r="D97">
-        <v>0</v>
-      </c>
-      <c r="E97">
+      <c r="B97" s="4">
+        <v>0</v>
+      </c>
+      <c r="C97" s="4">
+        <v>0</v>
+      </c>
+      <c r="D97" s="4">
+        <v>0</v>
+      </c>
+      <c r="E97" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3497,7 +3504,7 @@
       <c r="A101" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I101">
+      <c r="I101" s="4">
         <v>0</v>
       </c>
       <c r="J101" s="3">
@@ -3508,7 +3515,7 @@
       <c r="A102" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G102">
+      <c r="G102" s="4">
         <v>0</v>
       </c>
       <c r="H102" s="3">
@@ -3517,7 +3524,7 @@
       <c r="I102" s="3">
         <v>2</v>
       </c>
-      <c r="J102">
+      <c r="J102" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3585,7 +3592,7 @@
       <c r="I106" s="3">
         <v>2.0099999999999998</v>
       </c>
-      <c r="J106">
+      <c r="J106" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3602,7 +3609,7 @@
       <c r="I107" s="3">
         <v>4.66</v>
       </c>
-      <c r="J107">
+      <c r="J107" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3670,7 +3677,7 @@
       <c r="I111" s="3">
         <v>5.68</v>
       </c>
-      <c r="J111">
+      <c r="J111" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3687,7 +3694,7 @@
       <c r="I112" s="3">
         <v>2.17</v>
       </c>
-      <c r="J112">
+      <c r="J112" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3701,7 +3708,7 @@
       <c r="H113" s="3">
         <v>8.7100000000000009</v>
       </c>
-      <c r="I113">
+      <c r="I113" s="4">
         <v>0</v>
       </c>
       <c r="J113" s="3">
@@ -3820,10 +3827,10 @@
       <c r="H120" s="3">
         <v>0.38</v>
       </c>
-      <c r="I120">
-        <v>0</v>
-      </c>
-      <c r="J120">
+      <c r="I120" s="4">
+        <v>0</v>
+      </c>
+      <c r="J120" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3831,16 +3838,16 @@
       <c r="A121" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G121">
-        <v>0</v>
-      </c>
-      <c r="H121">
-        <v>0</v>
-      </c>
-      <c r="I121">
-        <v>0</v>
-      </c>
-      <c r="J121">
+      <c r="G121" s="4">
+        <v>0</v>
+      </c>
+      <c r="H121" s="4">
+        <v>0</v>
+      </c>
+      <c r="I121" s="4">
+        <v>0</v>
+      </c>
+      <c r="J121" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3857,7 +3864,7 @@
       <c r="I122" s="3">
         <v>5.08</v>
       </c>
-      <c r="J122">
+      <c r="J122" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3925,7 +3932,7 @@
       <c r="I126" s="3">
         <v>5.52</v>
       </c>
-      <c r="J126">
+      <c r="J126" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3942,7 +3949,7 @@
       <c r="I127" s="3">
         <v>4</v>
       </c>
-      <c r="J127">
+      <c r="J127" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4010,7 +4017,7 @@
       <c r="I131" s="2">
         <v>-35.549999999999997</v>
       </c>
-      <c r="J131">
+      <c r="J131" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4044,7 +4051,7 @@
       <c r="I133" s="3">
         <v>1.43</v>
       </c>
-      <c r="J133">
+      <c r="J133" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4078,7 +4085,7 @@
       <c r="I135" s="3">
         <v>4.07</v>
       </c>
-      <c r="J135">
+      <c r="J135" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4231,7 +4238,7 @@
       <c r="I144" s="3">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J144">
+      <c r="J144" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4262,7 +4269,7 @@
       <c r="G146" s="3">
         <v>4.0599999999999996</v>
       </c>
-      <c r="H146">
+      <c r="H146" s="4">
         <v>0</v>
       </c>
       <c r="I146" s="3">
@@ -4344,13 +4351,13 @@
       <c r="G151" s="3">
         <v>0.6</v>
       </c>
-      <c r="H151">
-        <v>0</v>
-      </c>
-      <c r="I151">
-        <v>0</v>
-      </c>
-      <c r="J151">
+      <c r="H151" s="4">
+        <v>0</v>
+      </c>
+      <c r="I151" s="4">
+        <v>0</v>
+      </c>
+      <c r="J151" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4384,7 +4391,7 @@
       <c r="I153" s="3">
         <v>5.87</v>
       </c>
-      <c r="J153">
+      <c r="J153" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4418,7 +4425,7 @@
       <c r="I155" s="3">
         <v>1.86</v>
       </c>
-      <c r="J155">
+      <c r="J155" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4435,7 +4442,7 @@
       <c r="I156" s="3">
         <v>1.77</v>
       </c>
-      <c r="J156">
+      <c r="J156" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4452,7 +4459,7 @@
       <c r="I157" s="3">
         <v>1.31</v>
       </c>
-      <c r="J157">
+      <c r="J157" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4517,7 +4524,7 @@
       <c r="G161" s="3">
         <v>0.94</v>
       </c>
-      <c r="H161">
+      <c r="H161" s="4">
         <v>0</v>
       </c>
       <c r="I161" s="3">
@@ -4622,7 +4629,7 @@
       <c r="I167" s="3">
         <v>2.85</v>
       </c>
-      <c r="J167">
+      <c r="J167" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4639,7 +4646,7 @@
       <c r="I168" s="3">
         <v>2.0099999999999998</v>
       </c>
-      <c r="J168">
+      <c r="J168" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4673,7 +4680,7 @@
       <c r="I170" s="3">
         <v>3.04</v>
       </c>
-      <c r="J170">
+      <c r="J170" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4724,7 +4731,7 @@
       <c r="I173" s="3">
         <v>9.23</v>
       </c>
-      <c r="J173">
+      <c r="J173" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4732,16 +4739,16 @@
       <c r="A174" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="F174">
-        <v>0</v>
-      </c>
-      <c r="G174">
-        <v>0</v>
-      </c>
-      <c r="H174">
-        <v>0</v>
-      </c>
-      <c r="I174">
+      <c r="F174" s="4">
+        <v>0</v>
+      </c>
+      <c r="G174" s="4">
+        <v>0</v>
+      </c>
+      <c r="H174" s="4">
+        <v>0</v>
+      </c>
+      <c r="I174" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4792,7 +4799,7 @@
       <c r="I177" s="3">
         <v>1.02</v>
       </c>
-      <c r="J177">
+      <c r="J177" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4809,7 +4816,7 @@
       <c r="I178" s="3">
         <v>6.11</v>
       </c>
-      <c r="J178">
+      <c r="J178" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4894,7 +4901,7 @@
       <c r="I183" s="3">
         <v>1.1399999999999999</v>
       </c>
-      <c r="J183">
+      <c r="J183" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4928,7 +4935,7 @@
       <c r="I185" s="2">
         <v>-0.79</v>
       </c>
-      <c r="J185">
+      <c r="J185" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4936,16 +4943,16 @@
       <c r="A186" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G186">
-        <v>0</v>
-      </c>
-      <c r="H186">
-        <v>0</v>
-      </c>
-      <c r="I186">
-        <v>0</v>
-      </c>
-      <c r="J186">
+      <c r="G186" s="4">
+        <v>0</v>
+      </c>
+      <c r="H186" s="4">
+        <v>0</v>
+      </c>
+      <c r="I186" s="4">
+        <v>0</v>
+      </c>
+      <c r="J186" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4953,7 +4960,7 @@
       <c r="A187" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F187">
+      <c r="F187" s="4">
         <v>0</v>
       </c>
       <c r="G187" s="3">
@@ -5044,7 +5051,7 @@
       <c r="I192" s="2">
         <v>-1.21</v>
       </c>
-      <c r="J192">
+      <c r="J192" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5146,7 +5153,7 @@
       <c r="I198" s="3">
         <v>6.11</v>
       </c>
-      <c r="J198">
+      <c r="J198" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5171,10 +5178,10 @@
       <c r="A200" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="H200">
-        <v>0</v>
-      </c>
-      <c r="I200">
+      <c r="H200" s="4">
+        <v>0</v>
+      </c>
+      <c r="I200" s="4">
         <v>0</v>
       </c>
       <c r="J200" s="3">
@@ -5191,7 +5198,7 @@
       <c r="H201" s="3">
         <v>2.66</v>
       </c>
-      <c r="I201">
+      <c r="I201" s="4">
         <v>0</v>
       </c>
       <c r="J201" s="3">
@@ -5225,7 +5232,7 @@
       <c r="H203" s="3">
         <v>2.2799999999999998</v>
       </c>
-      <c r="I203">
+      <c r="I203" s="4">
         <v>0</v>
       </c>
       <c r="J203" s="3">
@@ -5287,16 +5294,16 @@
       <c r="A207" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="F207">
-        <v>0</v>
-      </c>
-      <c r="G207">
-        <v>0</v>
-      </c>
-      <c r="H207">
-        <v>0</v>
-      </c>
-      <c r="I207">
+      <c r="F207" s="4">
+        <v>0</v>
+      </c>
+      <c r="G207" s="4">
+        <v>0</v>
+      </c>
+      <c r="H207" s="4">
+        <v>0</v>
+      </c>
+      <c r="I207" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5313,7 +5320,7 @@
       <c r="I208" s="3">
         <v>8.5399999999999991</v>
       </c>
-      <c r="J208">
+      <c r="J208" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5381,7 +5388,7 @@
       <c r="J212" s="3">
         <v>3.19</v>
       </c>
-      <c r="K212">
+      <c r="K212" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5398,7 +5405,7 @@
       <c r="I213" s="3">
         <v>2.41</v>
       </c>
-      <c r="J213">
+      <c r="J213" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5483,7 +5490,7 @@
       <c r="I218" s="3">
         <v>15.87</v>
       </c>
-      <c r="J218">
+      <c r="J218" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5500,7 +5507,7 @@
       <c r="I219" s="3">
         <v>5.16</v>
       </c>
-      <c r="J219">
+      <c r="J219" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5627,16 +5634,16 @@
       <c r="A227" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G227">
-        <v>0</v>
-      </c>
-      <c r="H227">
-        <v>0</v>
-      </c>
-      <c r="I227">
-        <v>0</v>
-      </c>
-      <c r="J227">
+      <c r="G227" s="4">
+        <v>0</v>
+      </c>
+      <c r="H227" s="4">
+        <v>0</v>
+      </c>
+      <c r="I227" s="4">
+        <v>0</v>
+      </c>
+      <c r="J227" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5687,7 +5694,7 @@
       <c r="I230" s="3">
         <v>2.78</v>
       </c>
-      <c r="J230">
+      <c r="J230" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5695,16 +5702,16 @@
       <c r="A231" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G231">
-        <v>0</v>
-      </c>
-      <c r="H231">
+      <c r="G231" s="4">
+        <v>0</v>
+      </c>
+      <c r="H231" s="4">
         <v>0</v>
       </c>
       <c r="I231" s="3">
         <v>0.1</v>
       </c>
-      <c r="J231">
+      <c r="J231" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5806,7 +5813,7 @@
       <c r="I237" s="3">
         <v>4.41</v>
       </c>
-      <c r="J237">
+      <c r="J237" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5857,7 +5864,7 @@
       <c r="I240" s="3">
         <v>3.87</v>
       </c>
-      <c r="J240">
+      <c r="J240" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5871,10 +5878,10 @@
       <c r="G241" s="3">
         <v>6.36</v>
       </c>
-      <c r="H241">
-        <v>0</v>
-      </c>
-      <c r="I241">
+      <c r="H241" s="4">
+        <v>0</v>
+      </c>
+      <c r="I241" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5885,13 +5892,13 @@
       <c r="F242" s="3">
         <v>0.88</v>
       </c>
-      <c r="G242">
-        <v>0</v>
-      </c>
-      <c r="H242">
-        <v>0</v>
-      </c>
-      <c r="I242">
+      <c r="G242" s="4">
+        <v>0</v>
+      </c>
+      <c r="H242" s="4">
+        <v>0</v>
+      </c>
+      <c r="I242" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5959,7 +5966,7 @@
       <c r="I246" s="3">
         <v>11.62</v>
       </c>
-      <c r="J246">
+      <c r="J246" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6044,7 +6051,7 @@
       <c r="I251" s="3">
         <v>3.3</v>
       </c>
-      <c r="J251">
+      <c r="J251" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6112,7 +6119,7 @@
       <c r="I255" s="3">
         <v>3.36</v>
       </c>
-      <c r="J255">
+      <c r="J255" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6154,7 +6161,7 @@
       <c r="A258" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="F258">
+      <c r="F258" s="4">
         <v>0</v>
       </c>
       <c r="G258" s="3">
@@ -6180,7 +6187,7 @@
       <c r="I259" s="3">
         <v>1.03</v>
       </c>
-      <c r="J259">
+      <c r="J259" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6350,7 +6357,7 @@
       <c r="I269" s="3">
         <v>3.14</v>
       </c>
-      <c r="J269">
+      <c r="J269" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6401,7 +6408,7 @@
       <c r="I272" s="3">
         <v>7.72</v>
       </c>
-      <c r="J272">
+      <c r="J272" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6409,16 +6416,16 @@
       <c r="A273" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="F273">
-        <v>0</v>
-      </c>
-      <c r="G273">
-        <v>0</v>
-      </c>
-      <c r="H273">
-        <v>0</v>
-      </c>
-      <c r="I273">
+      <c r="F273" s="4">
+        <v>0</v>
+      </c>
+      <c r="G273" s="4">
+        <v>0</v>
+      </c>
+      <c r="H273" s="4">
+        <v>0</v>
+      </c>
+      <c r="I273" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6469,7 +6476,7 @@
       <c r="I276" s="3">
         <v>2.79</v>
       </c>
-      <c r="J276">
+      <c r="J276" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6571,7 +6578,7 @@
       <c r="I282" s="3">
         <v>12.75</v>
       </c>
-      <c r="J282">
+      <c r="J282" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6616,7 +6623,7 @@
       <c r="H285" s="3">
         <v>2.4900000000000002</v>
       </c>
-      <c r="I285">
+      <c r="I285" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6624,7 +6631,7 @@
       <c r="A286" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="G286">
+      <c r="G286" s="4">
         <v>0</v>
       </c>
       <c r="H286" s="3">
@@ -6647,7 +6654,7 @@
       <c r="I287" s="2">
         <v>-6.07</v>
       </c>
-      <c r="J287">
+      <c r="J287" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6715,7 +6722,7 @@
       <c r="I291" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J291">
+      <c r="J291" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6740,13 +6747,13 @@
       <c r="A293" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="G293">
-        <v>0</v>
-      </c>
-      <c r="H293">
-        <v>0</v>
-      </c>
-      <c r="I293">
+      <c r="G293" s="4">
+        <v>0</v>
+      </c>
+      <c r="H293" s="4">
+        <v>0</v>
+      </c>
+      <c r="I293" s="4">
         <v>0</v>
       </c>
       <c r="J293" s="3">
@@ -6766,7 +6773,7 @@
       <c r="I294" s="3">
         <v>1.55</v>
       </c>
-      <c r="J294">
+      <c r="J294" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6800,7 +6807,7 @@
       <c r="I296" s="3">
         <v>5.13</v>
       </c>
-      <c r="J296">
+      <c r="J296" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6893,16 +6900,16 @@
       <c r="A302" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G302">
-        <v>0</v>
-      </c>
-      <c r="H302">
-        <v>0</v>
-      </c>
-      <c r="I302">
-        <v>0</v>
-      </c>
-      <c r="J302">
+      <c r="G302" s="4">
+        <v>0</v>
+      </c>
+      <c r="H302" s="4">
+        <v>0</v>
+      </c>
+      <c r="I302" s="4">
+        <v>0</v>
+      </c>
+      <c r="J302" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6910,7 +6917,7 @@
       <c r="A303" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="G303">
+      <c r="G303" s="4">
         <v>0</v>
       </c>
       <c r="H303" s="3">
@@ -6970,7 +6977,7 @@
       <c r="I306" s="3">
         <v>4.43</v>
       </c>
-      <c r="J306">
+      <c r="J306" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7089,7 +7096,7 @@
       <c r="I313" s="3">
         <v>1.81</v>
       </c>
-      <c r="J313">
+      <c r="J313" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7157,7 +7164,7 @@
       <c r="I317" s="3">
         <v>3.71</v>
       </c>
-      <c r="J317">
+      <c r="J317" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7191,7 +7198,7 @@
       <c r="I319" s="3">
         <v>4.1100000000000003</v>
       </c>
-      <c r="J319">
+      <c r="J319" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7199,16 +7206,16 @@
       <c r="A320" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="G320">
-        <v>0</v>
-      </c>
-      <c r="H320">
-        <v>0</v>
-      </c>
-      <c r="I320">
-        <v>0</v>
-      </c>
-      <c r="J320">
+      <c r="G320" s="4">
+        <v>0</v>
+      </c>
+      <c r="H320" s="4">
+        <v>0</v>
+      </c>
+      <c r="I320" s="4">
+        <v>0</v>
+      </c>
+      <c r="J320" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7259,7 +7266,7 @@
       <c r="I323" s="3">
         <v>1.38</v>
       </c>
-      <c r="J323">
+      <c r="J323" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7293,7 +7300,7 @@
       <c r="I325" s="3">
         <v>4.42</v>
       </c>
-      <c r="J325">
+      <c r="J325" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7361,7 +7368,7 @@
       <c r="I329" s="3">
         <v>5.18</v>
       </c>
-      <c r="J329">
+      <c r="J329" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7471,13 +7478,13 @@
       <c r="A336" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="H336">
+      <c r="H336" s="4">
         <v>0</v>
       </c>
       <c r="I336" s="3">
         <v>1</v>
       </c>
-      <c r="J336">
+      <c r="J336" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7502,7 +7509,7 @@
       <c r="A338" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="H338">
+      <c r="H338" s="4">
         <v>0</v>
       </c>
       <c r="I338" s="3">
@@ -7525,7 +7532,7 @@
       <c r="I339" s="3">
         <v>5.75</v>
       </c>
-      <c r="J339">
+      <c r="J339" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7559,7 +7566,7 @@
       <c r="I341" s="3">
         <v>6.17</v>
       </c>
-      <c r="J341">
+      <c r="J341" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7576,7 +7583,7 @@
       <c r="I342" s="3">
         <v>2.72</v>
       </c>
-      <c r="J342">
+      <c r="J342" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7618,16 +7625,16 @@
       <c r="A345" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="G345" s="3">
+      <c r="G345">
         <v>5.43</v>
       </c>
-      <c r="H345" s="3">
+      <c r="H345">
         <v>5.98</v>
       </c>
-      <c r="I345" s="3">
+      <c r="I345">
         <v>6.15</v>
       </c>
-      <c r="J345" s="3">
+      <c r="J345">
         <v>5.6</v>
       </c>
     </row>
@@ -7635,16 +7642,16 @@
       <c r="A346" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="F346" s="3">
+      <c r="F346">
         <v>4.95</v>
       </c>
-      <c r="G346" s="3">
+      <c r="G346">
         <v>5.43</v>
       </c>
-      <c r="H346" s="3">
+      <c r="H346">
         <v>6.47</v>
       </c>
-      <c r="I346" s="3">
+      <c r="I346">
         <v>6.92</v>
       </c>
     </row>
@@ -7652,16 +7659,16 @@
       <c r="A347" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="G347" s="3">
+      <c r="G347">
         <v>3.59</v>
       </c>
-      <c r="H347" s="3">
+      <c r="H347">
         <v>3.93</v>
       </c>
-      <c r="I347" s="3">
+      <c r="I347">
         <v>4.47</v>
       </c>
-      <c r="J347" s="3">
+      <c r="J347">
         <v>2.5299999999999998</v>
       </c>
     </row>
@@ -7669,16 +7676,16 @@
       <c r="A348" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="F348" s="3">
+      <c r="F348">
         <v>0.08</v>
       </c>
-      <c r="G348" s="3">
+      <c r="G348">
         <v>0.71</v>
       </c>
-      <c r="H348" s="3">
+      <c r="H348">
         <v>3.81</v>
       </c>
-      <c r="I348" s="2">
+      <c r="I348">
         <v>-4.29</v>
       </c>
     </row>
@@ -7686,13 +7693,13 @@
       <c r="A349" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="G349" s="3">
+      <c r="G349">
         <v>1.63</v>
       </c>
-      <c r="H349" s="3">
+      <c r="H349">
         <v>1.54</v>
       </c>
-      <c r="I349" s="3">
+      <c r="I349">
         <v>2.14</v>
       </c>
       <c r="J349">
@@ -7703,16 +7710,16 @@
       <c r="A350" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="G350" s="3">
+      <c r="G350">
         <v>0.01</v>
       </c>
-      <c r="H350" s="3">
+      <c r="H350">
         <v>2.75</v>
       </c>
-      <c r="I350" s="3">
+      <c r="I350">
         <v>1.84</v>
       </c>
-      <c r="J350" s="3">
+      <c r="J350">
         <v>1.91</v>
       </c>
     </row>
@@ -7720,16 +7727,16 @@
       <c r="A351" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="F351" s="3">
+      <c r="F351">
         <v>3.2</v>
       </c>
-      <c r="G351" s="3">
+      <c r="G351">
         <v>3.4</v>
       </c>
-      <c r="H351" s="3">
+      <c r="H351">
         <v>3.79</v>
       </c>
-      <c r="I351" s="3">
+      <c r="I351">
         <v>5.22</v>
       </c>
     </row>
@@ -7737,16 +7744,16 @@
       <c r="A352" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="F352" s="3">
+      <c r="F352">
         <v>0.69</v>
       </c>
-      <c r="G352" s="3">
+      <c r="G352">
         <v>0.78</v>
       </c>
-      <c r="H352" s="3">
+      <c r="H352">
         <v>0.96</v>
       </c>
-      <c r="I352" s="3">
+      <c r="I352">
         <v>1.04</v>
       </c>
     </row>
@@ -7754,16 +7761,16 @@
       <c r="A353" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="F353" s="3">
+      <c r="F353">
         <v>1.44</v>
       </c>
-      <c r="G353" s="3">
+      <c r="G353">
         <v>1.55</v>
       </c>
-      <c r="H353" s="3">
+      <c r="H353">
         <v>1.61</v>
       </c>
-      <c r="I353" s="3">
+      <c r="I353">
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -7771,13 +7778,13 @@
       <c r="A354" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="G354" s="3">
+      <c r="G354">
         <v>0.64</v>
       </c>
-      <c r="H354" s="3">
+      <c r="H354">
         <v>1.22</v>
       </c>
-      <c r="I354" s="3">
+      <c r="I354">
         <v>1.63</v>
       </c>
       <c r="J354">
@@ -7788,16 +7795,16 @@
       <c r="A355" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="F355" s="3">
+      <c r="F355">
         <v>6.15</v>
       </c>
-      <c r="G355" s="3">
+      <c r="G355">
         <v>7.41</v>
       </c>
-      <c r="H355" s="3">
+      <c r="H355">
         <v>8.9499999999999993</v>
       </c>
-      <c r="I355" s="3">
+      <c r="I355">
         <v>11.38</v>
       </c>
     </row>
@@ -7805,16 +7812,16 @@
       <c r="A356" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="G356" s="3">
+      <c r="G356">
         <v>4.37</v>
       </c>
-      <c r="H356" s="3">
+      <c r="H356">
         <v>4.59</v>
       </c>
       <c r="I356">
         <v>0</v>
       </c>
-      <c r="J356" s="3">
+      <c r="J356">
         <v>5.89</v>
       </c>
     </row>
@@ -7822,16 +7829,16 @@
       <c r="A357" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="G357" s="3">
+      <c r="G357">
         <v>5</v>
       </c>
-      <c r="H357" s="3">
+      <c r="H357">
         <v>5.42</v>
       </c>
-      <c r="I357" s="3">
+      <c r="I357">
         <v>3.33</v>
       </c>
-      <c r="J357" s="3">
+      <c r="J357">
         <v>5.77</v>
       </c>
     </row>
@@ -7839,16 +7846,16 @@
       <c r="A358" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="F358" s="3">
+      <c r="F358">
         <v>1.75</v>
       </c>
-      <c r="G358" s="3">
+      <c r="G358">
         <v>0.39</v>
       </c>
-      <c r="H358" s="3">
+      <c r="H358">
         <v>0.59</v>
       </c>
-      <c r="I358" s="3">
+      <c r="I358">
         <v>1.02</v>
       </c>
     </row>
@@ -7859,10 +7866,10 @@
       <c r="G359">
         <v>0</v>
       </c>
-      <c r="I359" s="3">
+      <c r="I359">
         <v>7.26</v>
       </c>
-      <c r="J359" s="3">
+      <c r="J359">
         <v>8.24</v>
       </c>
     </row>
@@ -7870,16 +7877,16 @@
       <c r="A360" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="F360" s="3">
+      <c r="F360">
         <v>4.4800000000000004</v>
       </c>
-      <c r="G360" s="3">
+      <c r="G360">
         <v>3.43</v>
       </c>
-      <c r="H360" s="3">
+      <c r="H360">
         <v>3.86</v>
       </c>
-      <c r="I360" s="3">
+      <c r="I360">
         <v>4.68</v>
       </c>
     </row>
@@ -7887,16 +7894,16 @@
       <c r="A361" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="F361" s="3">
+      <c r="F361">
         <v>2.7</v>
       </c>
-      <c r="G361" s="3">
+      <c r="G361">
         <v>1.88</v>
       </c>
-      <c r="H361" s="3">
+      <c r="H361">
         <v>2.19</v>
       </c>
-      <c r="I361" s="3">
+      <c r="I361">
         <v>2.6</v>
       </c>
     </row>
@@ -7904,16 +7911,16 @@
       <c r="A362" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="F362" s="3">
+      <c r="F362">
         <v>4.72</v>
       </c>
-      <c r="G362" s="3">
+      <c r="G362">
         <v>4.24</v>
       </c>
-      <c r="H362" s="3">
+      <c r="H362">
         <v>4.5199999999999996</v>
       </c>
-      <c r="I362" s="3">
+      <c r="I362">
         <v>5.88</v>
       </c>
     </row>
@@ -7921,13 +7928,13 @@
       <c r="A363" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="G363" s="3">
+      <c r="G363">
         <v>5.01</v>
       </c>
-      <c r="H363" s="2">
+      <c r="H363">
         <v>-0.42</v>
       </c>
-      <c r="I363" s="3">
+      <c r="I363">
         <v>4.26</v>
       </c>
       <c r="J363">
@@ -7938,16 +7945,16 @@
       <c r="A364" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="G364" s="2">
+      <c r="G364">
         <v>-0.31</v>
       </c>
-      <c r="H364" s="3">
+      <c r="H364">
         <v>0.95</v>
       </c>
-      <c r="I364" s="3">
+      <c r="I364">
         <v>0.21</v>
       </c>
-      <c r="J364" s="3">
+      <c r="J364">
         <v>0.59</v>
       </c>
     </row>
@@ -7955,16 +7962,16 @@
       <c r="A365" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="F365" s="3">
+      <c r="F365">
         <v>3.14</v>
       </c>
-      <c r="G365" s="3">
+      <c r="G365">
         <v>3.62</v>
       </c>
-      <c r="H365" s="3">
+      <c r="H365">
         <v>3.84</v>
       </c>
-      <c r="I365" s="3">
+      <c r="I365">
         <v>3.02</v>
       </c>
     </row>
@@ -7972,16 +7979,16 @@
       <c r="A366" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="F366" s="3">
+      <c r="F366">
         <v>3.56</v>
       </c>
-      <c r="G366" s="3">
+      <c r="G366">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H366" s="3">
+      <c r="H366">
         <v>4.72</v>
       </c>
-      <c r="I366" s="3">
+      <c r="I366">
         <v>5.43</v>
       </c>
     </row>
@@ -7989,16 +7996,16 @@
       <c r="A367" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="F367" s="3">
+      <c r="F367">
         <v>3.62</v>
       </c>
-      <c r="G367" s="3">
+      <c r="G367">
         <v>2.4300000000000002</v>
       </c>
-      <c r="H367" s="3">
+      <c r="H367">
         <v>3.26</v>
       </c>
-      <c r="I367" s="3">
+      <c r="I367">
         <v>3.62</v>
       </c>
     </row>
@@ -8006,13 +8013,13 @@
       <c r="A368" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="G368" s="3">
+      <c r="G368">
         <v>4.71</v>
       </c>
-      <c r="H368" s="3">
+      <c r="H368">
         <v>4.6500000000000004</v>
       </c>
-      <c r="I368" s="3">
+      <c r="I368">
         <v>4.53</v>
       </c>
       <c r="J368">
@@ -8023,16 +8030,16 @@
       <c r="A369" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="G369" s="3">
+      <c r="G369">
         <v>4.97</v>
       </c>
-      <c r="H369" s="3">
+      <c r="H369">
         <v>4.66</v>
       </c>
-      <c r="I369" s="3">
+      <c r="I369">
         <v>5.38</v>
       </c>
-      <c r="J369" s="3">
+      <c r="J369">
         <v>0.83</v>
       </c>
     </row>
@@ -8057,13 +8064,13 @@
       <c r="A371" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="G371" s="3">
+      <c r="G371">
         <v>3.16</v>
       </c>
       <c r="I371">
         <v>0</v>
       </c>
-      <c r="J371" s="3">
+      <c r="J371">
         <v>5.96</v>
       </c>
     </row>
@@ -8071,16 +8078,16 @@
       <c r="A372" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="G372" s="3">
+      <c r="G372">
         <v>1.48</v>
       </c>
-      <c r="H372" s="3">
+      <c r="H372">
         <v>2.44</v>
       </c>
-      <c r="I372" s="3">
+      <c r="I372">
         <v>4.21</v>
       </c>
-      <c r="J372" s="3">
+      <c r="J372">
         <v>5.27</v>
       </c>
     </row>
@@ -8088,13 +8095,13 @@
       <c r="A373" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="F373" s="2">
+      <c r="F373">
         <v>-2.0299999999999998</v>
       </c>
-      <c r="G373" s="3">
+      <c r="G373">
         <v>2.0099999999999998</v>
       </c>
-      <c r="H373" s="3">
+      <c r="H373">
         <v>2.63</v>
       </c>
       <c r="I373">
@@ -8111,10 +8118,10 @@
       <c r="G374">
         <v>0</v>
       </c>
-      <c r="H374" s="3">
+      <c r="H374">
         <v>2.78</v>
       </c>
-      <c r="I374" s="3">
+      <c r="I374">
         <v>2.66</v>
       </c>
     </row>
@@ -8122,13 +8129,13 @@
       <c r="A375" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="G375" s="3">
+      <c r="G375">
         <v>2.66</v>
       </c>
-      <c r="H375" s="3">
+      <c r="H375">
         <v>1.36</v>
       </c>
-      <c r="I375" s="3">
+      <c r="I375">
         <v>3.82</v>
       </c>
       <c r="J375">
@@ -8139,16 +8146,16 @@
       <c r="A376" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="G376" s="3">
+      <c r="G376">
         <v>1.0900000000000001</v>
       </c>
-      <c r="H376" s="3">
+      <c r="H376">
         <v>1.29</v>
       </c>
-      <c r="I376" s="3">
+      <c r="I376">
         <v>1.27</v>
       </c>
-      <c r="J376" s="3">
+      <c r="J376">
         <v>3.71</v>
       </c>
     </row>
@@ -8156,16 +8163,16 @@
       <c r="A377" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="G377" s="3">
+      <c r="G377">
         <v>1.68</v>
       </c>
-      <c r="H377" s="3">
+      <c r="H377">
         <v>1.59</v>
       </c>
-      <c r="I377" s="3">
+      <c r="I377">
         <v>1.1599999999999999</v>
       </c>
-      <c r="J377" s="3">
+      <c r="J377">
         <v>1.66</v>
       </c>
     </row>
@@ -8173,16 +8180,16 @@
       <c r="A378" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F378" s="3">
+      <c r="F378">
         <v>1.25</v>
       </c>
-      <c r="G378" s="3">
+      <c r="G378">
         <v>3.39</v>
       </c>
-      <c r="H378" s="3">
+      <c r="H378">
         <v>1.19</v>
       </c>
-      <c r="I378" s="3">
+      <c r="I378">
         <v>2.37</v>
       </c>
     </row>
@@ -8190,13 +8197,13 @@
       <c r="A379" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="G379" s="3">
+      <c r="G379">
         <v>3.1</v>
       </c>
-      <c r="H379" s="3">
+      <c r="H379">
         <v>2.78</v>
       </c>
-      <c r="I379" s="3">
+      <c r="I379">
         <v>1.94</v>
       </c>
       <c r="J379">
@@ -8207,16 +8214,16 @@
       <c r="A380" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="F380" s="3">
+      <c r="F380">
         <v>2.4900000000000002</v>
       </c>
-      <c r="G380" s="3">
+      <c r="G380">
         <v>2.31</v>
       </c>
-      <c r="H380" s="3">
+      <c r="H380">
         <v>2.36</v>
       </c>
-      <c r="I380" s="2">
+      <c r="I380">
         <v>-1.53</v>
       </c>
     </row>
@@ -8224,16 +8231,16 @@
       <c r="A381" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="G381" s="2">
+      <c r="G381">
         <v>-0.2</v>
       </c>
-      <c r="H381" s="3">
+      <c r="H381">
         <v>1.91</v>
       </c>
-      <c r="I381" s="3">
+      <c r="I381">
         <v>2.5</v>
       </c>
-      <c r="J381" s="3">
+      <c r="J381">
         <v>2.77</v>
       </c>
     </row>
@@ -8241,16 +8248,16 @@
       <c r="A382" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="G382" s="3">
+      <c r="G382">
         <v>3.05</v>
       </c>
-      <c r="H382" s="3">
+      <c r="H382">
         <v>4.34</v>
       </c>
-      <c r="I382" s="3">
+      <c r="I382">
         <v>5.98</v>
       </c>
-      <c r="J382" s="3">
+      <c r="J382">
         <v>5.49</v>
       </c>
     </row>
@@ -8258,16 +8265,16 @@
       <c r="A383" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="F383" s="3">
+      <c r="F383">
         <v>1.83</v>
       </c>
-      <c r="G383" s="3">
+      <c r="G383">
         <v>1.7</v>
       </c>
       <c r="H383">
         <v>0</v>
       </c>
-      <c r="I383" s="3">
+      <c r="I383">
         <v>2.04</v>
       </c>
     </row>
@@ -8275,16 +8282,16 @@
       <c r="A384" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="G384" s="3">
+      <c r="G384">
         <v>4.57</v>
       </c>
-      <c r="H384" s="3">
+      <c r="H384">
         <v>3.1</v>
       </c>
-      <c r="I384" s="2">
+      <c r="I384">
         <v>-2.58</v>
       </c>
-      <c r="J384" s="3">
+      <c r="J384">
         <v>5.35</v>
       </c>
     </row>
@@ -8292,16 +8299,16 @@
       <c r="A385" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="G385" s="3">
+      <c r="G385">
         <v>3.28</v>
       </c>
-      <c r="H385" s="3">
+      <c r="H385">
         <v>1.42</v>
       </c>
-      <c r="I385" s="3">
+      <c r="I385">
         <v>3.75</v>
       </c>
-      <c r="J385" s="3">
+      <c r="J385">
         <v>3.61</v>
       </c>
     </row>
@@ -8309,16 +8316,16 @@
       <c r="A386" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="G386" s="3">
+      <c r="G386">
         <v>2.6</v>
       </c>
-      <c r="H386" s="3">
+      <c r="H386">
         <v>3</v>
       </c>
-      <c r="I386" s="3">
+      <c r="I386">
         <v>3.2</v>
       </c>
-      <c r="J386" s="3">
+      <c r="J386">
         <v>3.38</v>
       </c>
     </row>
@@ -8326,16 +8333,16 @@
       <c r="A387" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="F387" s="3">
+      <c r="F387">
         <v>5.48</v>
       </c>
-      <c r="G387" s="3">
+      <c r="G387">
         <v>5.76</v>
       </c>
-      <c r="H387" s="3">
+      <c r="H387">
         <v>4.1500000000000004</v>
       </c>
-      <c r="I387" s="3">
+      <c r="I387">
         <v>4.21</v>
       </c>
     </row>
@@ -8343,16 +8350,16 @@
       <c r="A388" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="F388" s="3">
+      <c r="F388">
         <v>3.24</v>
       </c>
-      <c r="G388" s="3">
+      <c r="G388">
         <v>3.53</v>
       </c>
-      <c r="H388" s="3">
+      <c r="H388">
         <v>4.76</v>
       </c>
-      <c r="I388" s="3">
+      <c r="I388">
         <v>4.96</v>
       </c>
     </row>
@@ -8360,16 +8367,16 @@
       <c r="A389" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="F389" s="3">
+      <c r="F389">
         <v>1.39</v>
       </c>
-      <c r="G389" s="3">
+      <c r="G389">
         <v>1.44</v>
       </c>
-      <c r="H389" s="3">
+      <c r="H389">
         <v>1.58</v>
       </c>
-      <c r="I389" s="3">
+      <c r="I389">
         <v>1.38</v>
       </c>
     </row>
@@ -8377,13 +8384,13 @@
       <c r="A390" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="G390" s="3">
+      <c r="G390">
         <v>9.84</v>
       </c>
-      <c r="H390" s="3">
+      <c r="H390">
         <v>10.82</v>
       </c>
-      <c r="I390" s="3">
+      <c r="I390">
         <v>10.99</v>
       </c>
       <c r="J390">
@@ -8394,16 +8401,16 @@
       <c r="A391" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="F391" s="3">
+      <c r="F391">
         <v>3.89</v>
       </c>
-      <c r="G391" s="3">
+      <c r="G391">
         <v>2.35</v>
       </c>
-      <c r="H391" s="3">
+      <c r="H391">
         <v>2.69</v>
       </c>
-      <c r="I391" s="3">
+      <c r="I391">
         <v>3.03</v>
       </c>
     </row>
@@ -8428,16 +8435,16 @@
       <c r="A393" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="F393" s="3">
+      <c r="F393">
         <v>5.33</v>
       </c>
-      <c r="G393" s="3">
+      <c r="G393">
         <v>3.05</v>
       </c>
-      <c r="H393" s="3">
+      <c r="H393">
         <v>6.56</v>
       </c>
-      <c r="I393" s="3">
+      <c r="I393">
         <v>12.5</v>
       </c>
     </row>
@@ -8445,16 +8452,16 @@
       <c r="A394" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="F394" s="3">
+      <c r="F394">
         <v>1.3</v>
       </c>
-      <c r="G394" s="3">
+      <c r="G394">
         <v>1.3</v>
       </c>
-      <c r="H394" s="3">
+      <c r="H394">
         <v>1.73</v>
       </c>
-      <c r="I394" s="3">
+      <c r="I394">
         <v>1.98</v>
       </c>
     </row>
@@ -8462,16 +8469,16 @@
       <c r="A395" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="F395" s="3">
+      <c r="F395">
         <v>1.53</v>
       </c>
-      <c r="G395" s="3">
+      <c r="G395">
         <v>1.94</v>
       </c>
-      <c r="H395" s="3">
+      <c r="H395">
         <v>2.61</v>
       </c>
-      <c r="I395" s="3">
+      <c r="I395">
         <v>2.86</v>
       </c>
     </row>
@@ -8479,16 +8486,16 @@
       <c r="A396" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="F396" s="3">
+      <c r="F396">
         <v>2.1</v>
       </c>
-      <c r="G396" s="3">
+      <c r="G396">
         <v>1.78</v>
       </c>
-      <c r="I396" s="3">
+      <c r="I396">
         <v>2.15</v>
       </c>
-      <c r="J396" s="3">
+      <c r="J396">
         <v>2.52</v>
       </c>
     </row>
@@ -8496,16 +8503,16 @@
       <c r="A397" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="F397" s="3">
+      <c r="F397">
         <v>1.23</v>
       </c>
-      <c r="G397" s="3">
+      <c r="G397">
         <v>1.54</v>
       </c>
-      <c r="H397" s="3">
+      <c r="H397">
         <v>0.98</v>
       </c>
-      <c r="I397" s="3">
+      <c r="I397">
         <v>1.08</v>
       </c>
     </row>
@@ -8530,16 +8537,16 @@
       <c r="A399" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="F399" s="2">
+      <c r="F399">
         <v>-2.1800000000000002</v>
       </c>
-      <c r="G399" s="3">
+      <c r="G399">
         <v>1.64</v>
       </c>
-      <c r="H399" s="3">
+      <c r="H399">
         <v>3.05</v>
       </c>
-      <c r="I399" s="3">
+      <c r="I399">
         <v>19.52</v>
       </c>
     </row>
@@ -8547,16 +8554,16 @@
       <c r="A400" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="F400" s="3">
+      <c r="F400">
         <v>0.85</v>
       </c>
-      <c r="G400" s="3">
+      <c r="G400">
         <v>0.16</v>
       </c>
-      <c r="H400" s="3">
+      <c r="H400">
         <v>0.6</v>
       </c>
-      <c r="I400" s="3">
+      <c r="I400">
         <v>1.3</v>
       </c>
     </row>
@@ -8564,16 +8571,16 @@
       <c r="A401" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="F401" s="3">
+      <c r="F401">
         <v>4.57</v>
       </c>
-      <c r="G401" s="3">
+      <c r="G401">
         <v>5.21</v>
       </c>
-      <c r="H401" s="3">
+      <c r="H401">
         <v>5.52</v>
       </c>
-      <c r="I401" s="3">
+      <c r="I401">
         <v>6.89</v>
       </c>
     </row>
@@ -8581,13 +8588,13 @@
       <c r="A402" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="G402" s="3">
+      <c r="G402">
         <v>2.73</v>
       </c>
       <c r="H402">
         <v>0</v>
       </c>
-      <c r="I402" s="3">
+      <c r="I402">
         <v>4</v>
       </c>
       <c r="J402">
@@ -8598,13 +8605,13 @@
       <c r="A403" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="G403" s="3">
+      <c r="G403">
         <v>5.59</v>
       </c>
-      <c r="H403" s="3">
+      <c r="H403">
         <v>5.78</v>
       </c>
-      <c r="I403" s="3">
+      <c r="I403">
         <v>6.1</v>
       </c>
       <c r="J403">
@@ -8615,16 +8622,16 @@
       <c r="A404" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="F404" s="3">
+      <c r="F404">
         <v>3.18</v>
       </c>
-      <c r="G404" s="3">
+      <c r="G404">
         <v>3.24</v>
       </c>
-      <c r="H404" s="3">
+      <c r="H404">
         <v>1.62</v>
       </c>
-      <c r="I404" s="3">
+      <c r="I404">
         <v>3.51</v>
       </c>
     </row>
@@ -8632,13 +8639,13 @@
       <c r="A405" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="G405" s="3">
+      <c r="G405">
         <v>9.4700000000000006</v>
       </c>
-      <c r="H405" s="3">
+      <c r="H405">
         <v>5.77</v>
       </c>
-      <c r="I405" s="3">
+      <c r="I405">
         <v>5.51</v>
       </c>
       <c r="J405">
@@ -8649,16 +8656,16 @@
       <c r="A406" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="F406" s="3">
+      <c r="F406">
         <v>0.84</v>
       </c>
-      <c r="G406" s="3">
+      <c r="G406">
         <v>4.6500000000000004</v>
       </c>
-      <c r="H406" s="3">
+      <c r="H406">
         <v>3.31</v>
       </c>
-      <c r="I406" s="3">
+      <c r="I406">
         <v>5.38</v>
       </c>
     </row>
@@ -8666,16 +8673,16 @@
       <c r="A407" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="G407" s="3">
+      <c r="G407">
         <v>1.63</v>
       </c>
-      <c r="H407" s="3">
+      <c r="H407">
         <v>1.92</v>
       </c>
-      <c r="I407" s="3">
+      <c r="I407">
         <v>1.7</v>
       </c>
-      <c r="J407" s="3">
+      <c r="J407">
         <v>1.79</v>
       </c>
     </row>
@@ -8700,13 +8707,13 @@
       <c r="A409" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="G409" s="3">
+      <c r="G409">
         <v>6.35</v>
       </c>
-      <c r="H409" s="3">
+      <c r="H409">
         <v>6.92</v>
       </c>
-      <c r="I409" s="3">
+      <c r="I409">
         <v>8.7200000000000006</v>
       </c>
       <c r="J409">
@@ -8734,16 +8741,16 @@
       <c r="A411" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="G411" s="3">
+      <c r="G411">
         <v>4.04</v>
       </c>
-      <c r="H411" s="3">
+      <c r="H411">
         <v>3.88</v>
       </c>
-      <c r="I411" s="3">
+      <c r="I411">
         <v>4.13</v>
       </c>
-      <c r="J411" s="3">
+      <c r="J411">
         <v>4.22</v>
       </c>
     </row>
@@ -8757,10 +8764,10 @@
       <c r="G412">
         <v>0</v>
       </c>
-      <c r="I412" s="3">
+      <c r="I412">
         <v>2.42</v>
       </c>
-      <c r="J412" s="3">
+      <c r="J412">
         <v>2.9</v>
       </c>
     </row>
@@ -8768,16 +8775,16 @@
       <c r="A413" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G413" s="3">
+      <c r="G413">
         <v>4.93</v>
       </c>
-      <c r="H413" s="3">
+      <c r="H413">
         <v>5.53</v>
       </c>
-      <c r="I413" s="3">
+      <c r="I413">
         <v>4.78</v>
       </c>
-      <c r="J413" s="3">
+      <c r="J413">
         <v>3.63</v>
       </c>
     </row>
@@ -8785,16 +8792,16 @@
       <c r="A414" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="F414" s="3">
+      <c r="F414">
         <v>3.77</v>
       </c>
-      <c r="G414" s="3">
+      <c r="G414">
         <v>4.99</v>
       </c>
-      <c r="H414" s="3">
+      <c r="H414">
         <v>6.88</v>
       </c>
-      <c r="I414" s="3">
+      <c r="I414">
         <v>8</v>
       </c>
     </row>
@@ -8802,16 +8809,16 @@
       <c r="A415" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="F415" s="2">
+      <c r="F415">
         <v>-0.41</v>
       </c>
-      <c r="G415" s="3">
+      <c r="G415">
         <v>0.19</v>
       </c>
-      <c r="H415" s="3">
+      <c r="H415">
         <v>1.56</v>
       </c>
-      <c r="I415" s="3">
+      <c r="I415">
         <v>1.66</v>
       </c>
     </row>
@@ -8819,13 +8826,13 @@
       <c r="A416" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="G416" s="3">
+      <c r="G416">
         <v>2.1</v>
       </c>
-      <c r="H416" s="3">
+      <c r="H416">
         <v>4.18</v>
       </c>
-      <c r="I416" s="3">
+      <c r="I416">
         <v>3.61</v>
       </c>
       <c r="J416">
@@ -8836,16 +8843,16 @@
       <c r="A417" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="F417" s="3">
+      <c r="F417">
         <v>1.98</v>
       </c>
-      <c r="G417" s="3">
+      <c r="G417">
         <v>2.0699999999999998</v>
       </c>
-      <c r="H417" s="3">
+      <c r="H417">
         <v>2.41</v>
       </c>
-      <c r="I417" s="3">
+      <c r="I417">
         <v>3.07</v>
       </c>
     </row>
@@ -8853,16 +8860,16 @@
       <c r="A418" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="F418" s="3">
+      <c r="F418">
         <v>2.04</v>
       </c>
-      <c r="G418" s="3">
+      <c r="G418">
         <v>3.77</v>
       </c>
-      <c r="H418" s="3">
+      <c r="H418">
         <v>2.8</v>
       </c>
-      <c r="I418" s="3">
+      <c r="I418">
         <v>3.29</v>
       </c>
     </row>
@@ -8870,16 +8877,16 @@
       <c r="A419" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="F419" s="2">
+      <c r="F419">
         <v>-0.5</v>
       </c>
-      <c r="G419" s="2">
+      <c r="G419">
         <v>-1.98</v>
       </c>
-      <c r="H419" s="2">
+      <c r="H419">
         <v>-3.14</v>
       </c>
-      <c r="I419" s="2">
+      <c r="I419">
         <v>-2.31</v>
       </c>
     </row>
@@ -8887,13 +8894,13 @@
       <c r="A420" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="G420" s="3">
+      <c r="G420">
         <v>1.55</v>
       </c>
-      <c r="H420" s="3">
+      <c r="H420">
         <v>1.62</v>
       </c>
-      <c r="I420" s="3">
+      <c r="I420">
         <v>1.26</v>
       </c>
       <c r="J420">
@@ -8904,16 +8911,16 @@
       <c r="A421" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="F421" s="3">
+      <c r="F421">
         <v>0.31</v>
       </c>
-      <c r="G421" s="3">
+      <c r="G421">
         <v>4.01</v>
       </c>
-      <c r="H421" s="3">
+      <c r="H421">
         <v>2.42</v>
       </c>
-      <c r="I421" s="3">
+      <c r="I421">
         <v>4.38</v>
       </c>
     </row>
@@ -8930,7 +8937,7 @@
       <c r="H422">
         <v>0</v>
       </c>
-      <c r="I422" s="3">
+      <c r="I422">
         <v>5.7</v>
       </c>
     </row>
@@ -8938,16 +8945,16 @@
       <c r="A423" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="G423" s="3">
+      <c r="G423">
         <v>4.07</v>
       </c>
-      <c r="H423" s="3">
+      <c r="H423">
         <v>6.88</v>
       </c>
-      <c r="I423" s="3">
+      <c r="I423">
         <v>6.31</v>
       </c>
-      <c r="J423" s="3">
+      <c r="J423">
         <v>1.01</v>
       </c>
     </row>
@@ -8955,16 +8962,16 @@
       <c r="A424" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="F424" s="3">
+      <c r="F424">
         <v>2.37</v>
       </c>
-      <c r="G424" s="3">
+      <c r="G424">
         <v>2.54</v>
       </c>
-      <c r="H424" s="3">
+      <c r="H424">
         <v>2.61</v>
       </c>
-      <c r="I424" s="3">
+      <c r="I424">
         <v>2.36</v>
       </c>
     </row>
@@ -8972,16 +8979,16 @@
       <c r="A425" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="F425" s="3">
+      <c r="F425">
         <v>3.4</v>
       </c>
-      <c r="G425" s="3">
+      <c r="G425">
         <v>3.95</v>
       </c>
-      <c r="H425" s="3">
+      <c r="H425">
         <v>4.17</v>
       </c>
-      <c r="I425" s="3">
+      <c r="I425">
         <v>4.18</v>
       </c>
     </row>
@@ -8989,16 +8996,16 @@
       <c r="A426" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="G426" s="3">
+      <c r="G426">
         <v>1.48</v>
       </c>
-      <c r="H426" s="3">
+      <c r="H426">
         <v>1.57</v>
       </c>
-      <c r="I426" s="3">
+      <c r="I426">
         <v>1.49</v>
       </c>
-      <c r="J426" s="3">
+      <c r="J426">
         <v>1.55</v>
       </c>
     </row>
@@ -9006,13 +9013,13 @@
       <c r="A427" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="G427" s="3">
+      <c r="G427">
         <v>10.42</v>
       </c>
-      <c r="H427" s="3">
+      <c r="H427">
         <v>8.3000000000000007</v>
       </c>
-      <c r="I427" s="3">
+      <c r="I427">
         <v>9.9499999999999993</v>
       </c>
       <c r="J427">
@@ -9040,13 +9047,13 @@
       <c r="A429" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="G429" s="3">
+      <c r="G429">
         <v>0.21</v>
       </c>
-      <c r="H429" s="3">
+      <c r="H429">
         <v>2.8</v>
       </c>
-      <c r="I429" s="3">
+      <c r="I429">
         <v>1.66</v>
       </c>
       <c r="J429">
@@ -9057,16 +9064,16 @@
       <c r="A430" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="F430" s="3">
+      <c r="F430">
         <v>1.39</v>
       </c>
-      <c r="G430" s="3">
+      <c r="G430">
         <v>0.63</v>
       </c>
-      <c r="H430" s="3">
+      <c r="H430">
         <v>2.94</v>
       </c>
-      <c r="I430" s="2">
+      <c r="I430">
         <v>-0.76</v>
       </c>
     </row>
@@ -9074,16 +9081,16 @@
       <c r="A431" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="G431" s="3">
+      <c r="G431">
         <v>5.04</v>
       </c>
-      <c r="H431" s="3">
+      <c r="H431">
         <v>4.9000000000000004</v>
       </c>
-      <c r="I431" s="3">
+      <c r="I431">
         <v>5.07</v>
       </c>
-      <c r="J431" s="3">
+      <c r="J431">
         <v>4.58</v>
       </c>
     </row>
@@ -9094,10 +9101,10 @@
       <c r="H432">
         <v>0</v>
       </c>
-      <c r="I432" s="3">
+      <c r="I432">
         <v>2.97</v>
       </c>
-      <c r="J432" s="2">
+      <c r="J432">
         <v>-1.56</v>
       </c>
     </row>
@@ -9105,16 +9112,16 @@
       <c r="A433" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="F433" s="3">
+      <c r="F433">
         <v>1.7</v>
       </c>
-      <c r="G433" s="3">
+      <c r="G433">
         <v>1.43</v>
       </c>
-      <c r="H433" s="3">
+      <c r="H433">
         <v>1.6</v>
       </c>
-      <c r="I433" s="3">
+      <c r="I433">
         <v>1.63</v>
       </c>
     </row>
@@ -9122,16 +9129,16 @@
       <c r="A434" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="F434" s="3">
+      <c r="F434">
         <v>0.71</v>
       </c>
-      <c r="G434" s="3">
+      <c r="G434">
         <v>0.95</v>
       </c>
-      <c r="H434" s="3">
+      <c r="H434">
         <v>3.2</v>
       </c>
-      <c r="I434" s="3">
+      <c r="I434">
         <v>0.89</v>
       </c>
     </row>
@@ -9139,16 +9146,16 @@
       <c r="A435" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="F435" s="3">
+      <c r="F435">
         <v>2.8</v>
       </c>
-      <c r="G435" s="3">
+      <c r="G435">
         <v>3.25</v>
       </c>
-      <c r="H435" s="3">
+      <c r="H435">
         <v>4.22</v>
       </c>
-      <c r="I435" s="3">
+      <c r="I435">
         <v>5.18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates - auto adjusted all column widths in all worksheets of workbooks
</commit_message>
<xml_diff>
--- a/earnings_per_share_pivot_table.xlsx
+++ b/earnings_per_share_pivot_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2869E2F4B8130AB5A65CD8CB5FEE27FB797A1921" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8904B0E-0D43-4A02-9310-A46B87F686B0}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2869E2F4B8130AB5A65CD8C0976D2CD7797A1921" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59A55633-F108-4686-97B8-9044151BF2E8}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
created nflx stock yearly earnings per share dataframe
</commit_message>
<xml_diff>
--- a/earnings_per_share_pivot_table.xlsx
+++ b/earnings_per_share_pivot_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2869E2F4B8130AB5A65CD88E3F6D1237797A1921" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F31E8DC-0934-4F1E-B41C-346D608CC56E}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2869E2F4B8130AB5A65CD882872E382D797A1921" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEE8391A-B303-4722-9069-38FA6AE0A21F}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
created nke stock yearly earnings per share dataframe
</commit_message>
<xml_diff>
--- a/earnings_per_share_pivot_table.xlsx
+++ b/earnings_per_share_pivot_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2869E2F4B8130AB5A65CD8BD07EE1001797A1921" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F0A3062-7F80-4CE9-AC5B-8672170A4C6C}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2869E2F4B8130AB5A65CD8B277E82D49797A1921" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10046C91-DB2E-422B-A898-518CACCD1C39}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>